<commit_message>
update and record answer
</commit_message>
<xml_diff>
--- a/third_party_feedback/feedback/data/eqlabels.xlsx
+++ b/third_party_feedback/feedback/data/eqlabels.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\code\github\abelit-ThirdParty\third_party_feedback\feedback\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D61E326-3808-4C1D-9AAC-CA609DB2FF93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD9C194-FC2D-4239-9236-E9F12287FB15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TTO" sheetId="1" r:id="rId1"/>
     <sheet name="TTO-Feedback" sheetId="2" r:id="rId2"/>
     <sheet name="DCE" sheetId="3" r:id="rId3"/>
     <sheet name="Open ended questions" sheetId="4" r:id="rId4"/>
+    <sheet name="Non-Stopping TTO" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="161">
   <si>
     <t>Presentation</t>
   </si>
@@ -509,14 +510,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>type</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>type</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>version</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -525,6 +518,10 @@
   </si>
   <si>
     <t>V17</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>questionid</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -1064,8 +1061,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G50"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1095,10 +1092,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="46" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" s="40" t="s">
         <v>157</v>
-      </c>
-      <c r="G1" s="40" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1121,7 +1118,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="40" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1144,7 +1141,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="40" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1167,7 +1164,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="31.5">
@@ -1190,7 +1187,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1213,7 +1210,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1236,7 +1233,7 @@
         <v>2</v>
       </c>
       <c r="G7" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1259,7 +1256,7 @@
         <v>2</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1282,7 +1279,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1305,7 +1302,7 @@
         <v>2</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1328,7 +1325,7 @@
         <v>2</v>
       </c>
       <c r="G11" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1351,7 +1348,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="31.5">
@@ -1374,7 +1371,7 @@
         <v>2</v>
       </c>
       <c r="G13" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1397,7 +1394,7 @@
         <v>2</v>
       </c>
       <c r="G14" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1420,7 +1417,7 @@
         <v>2</v>
       </c>
       <c r="G15" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1443,7 +1440,7 @@
         <v>2</v>
       </c>
       <c r="G16" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1466,7 +1463,7 @@
         <v>2</v>
       </c>
       <c r="G17" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1489,7 +1486,7 @@
         <v>2</v>
       </c>
       <c r="G18" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1512,7 +1509,7 @@
         <v>2</v>
       </c>
       <c r="G19" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1535,7 +1532,7 @@
         <v>2</v>
       </c>
       <c r="G20" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1558,7 +1555,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="31.5">
@@ -1581,7 +1578,7 @@
         <v>2</v>
       </c>
       <c r="G22" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1604,7 +1601,7 @@
         <v>2</v>
       </c>
       <c r="G23" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="31.5">
@@ -1627,7 +1624,7 @@
         <v>2</v>
       </c>
       <c r="G24" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1650,7 +1647,7 @@
         <v>2</v>
       </c>
       <c r="G25" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1673,7 +1670,7 @@
         <v>2</v>
       </c>
       <c r="G26" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1696,7 +1693,7 @@
         <v>2</v>
       </c>
       <c r="G27" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1719,7 +1716,7 @@
         <v>2</v>
       </c>
       <c r="G28" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="31.5">
@@ -1742,7 +1739,7 @@
         <v>2</v>
       </c>
       <c r="G29" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1765,7 +1762,7 @@
         <v>2</v>
       </c>
       <c r="G30" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="63">
@@ -1788,7 +1785,7 @@
         <v>2</v>
       </c>
       <c r="G31" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1811,7 +1808,7 @@
         <v>2</v>
       </c>
       <c r="G32" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1834,7 +1831,7 @@
         <v>2</v>
       </c>
       <c r="G33" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1857,7 +1854,7 @@
         <v>2</v>
       </c>
       <c r="G34" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1880,7 +1877,7 @@
         <v>2</v>
       </c>
       <c r="G35" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1903,7 +1900,7 @@
         <v>2</v>
       </c>
       <c r="G36" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1926,7 +1923,7 @@
         <v>2</v>
       </c>
       <c r="G37" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1949,7 +1946,7 @@
         <v>2</v>
       </c>
       <c r="G38" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1972,7 +1969,7 @@
         <v>2</v>
       </c>
       <c r="G39" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1995,7 +1992,7 @@
         <v>2</v>
       </c>
       <c r="G40" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -2018,7 +2015,7 @@
         <v>2</v>
       </c>
       <c r="G41" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -2041,7 +2038,7 @@
         <v>2</v>
       </c>
       <c r="G42" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -2064,7 +2061,7 @@
         <v>2</v>
       </c>
       <c r="G43" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="31.5">
@@ -2087,7 +2084,7 @@
         <v>2</v>
       </c>
       <c r="G44" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -2110,7 +2107,7 @@
         <v>2</v>
       </c>
       <c r="G45" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="47.25">
@@ -2133,7 +2130,7 @@
         <v>2</v>
       </c>
       <c r="G46" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="63">
@@ -2156,7 +2153,7 @@
         <v>2</v>
       </c>
       <c r="G47" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -2179,7 +2176,7 @@
         <v>2</v>
       </c>
       <c r="G48" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -2202,7 +2199,7 @@
         <v>2</v>
       </c>
       <c r="G49" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -2225,7 +2222,7 @@
         <v>2</v>
       </c>
       <c r="G50" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2336,8 +2333,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -2367,10 +2364,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" s="40" t="s">
         <v>157</v>
-      </c>
-      <c r="G1" s="40" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2393,7 +2390,7 @@
         <v>3</v>
       </c>
       <c r="G2" s="40" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2416,7 +2413,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="40" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2439,7 +2436,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="31.5">
@@ -2462,7 +2459,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2485,7 +2482,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2508,7 +2505,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2531,7 +2528,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -2554,7 +2551,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2577,7 +2574,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -2600,7 +2597,7 @@
         <v>3</v>
       </c>
       <c r="G11" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -2623,7 +2620,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="31.5">
@@ -2646,7 +2643,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2669,7 +2666,7 @@
         <v>3</v>
       </c>
       <c r="G14" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2692,7 +2689,7 @@
         <v>3</v>
       </c>
       <c r="G15" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -2715,7 +2712,7 @@
         <v>3</v>
       </c>
       <c r="G16" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -2738,7 +2735,7 @@
         <v>3</v>
       </c>
       <c r="G17" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -2761,7 +2758,7 @@
         <v>3</v>
       </c>
       <c r="G18" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -2784,7 +2781,7 @@
         <v>3</v>
       </c>
       <c r="G19" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -2807,7 +2804,7 @@
         <v>3</v>
       </c>
       <c r="G20" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -2830,7 +2827,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="31.5">
@@ -2853,7 +2850,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -2876,7 +2873,7 @@
         <v>3</v>
       </c>
       <c r="G23" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="31.5">
@@ -2899,7 +2896,7 @@
         <v>3</v>
       </c>
       <c r="G24" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -2922,7 +2919,7 @@
         <v>3</v>
       </c>
       <c r="G25" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -2945,7 +2942,7 @@
         <v>3</v>
       </c>
       <c r="G26" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -2968,7 +2965,7 @@
         <v>3</v>
       </c>
       <c r="G27" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -2991,7 +2988,7 @@
         <v>3</v>
       </c>
       <c r="G28" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="31.5">
@@ -3014,7 +3011,7 @@
         <v>3</v>
       </c>
       <c r="G29" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -3037,7 +3034,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="63">
@@ -3060,7 +3057,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -3083,7 +3080,7 @@
         <v>3</v>
       </c>
       <c r="G32" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -3106,7 +3103,7 @@
         <v>3</v>
       </c>
       <c r="G33" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -3129,7 +3126,7 @@
         <v>3</v>
       </c>
       <c r="G34" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -3152,7 +3149,7 @@
         <v>3</v>
       </c>
       <c r="G35" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -3175,7 +3172,7 @@
         <v>3</v>
       </c>
       <c r="G36" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -3198,7 +3195,7 @@
         <v>3</v>
       </c>
       <c r="G37" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -3221,7 +3218,7 @@
         <v>3</v>
       </c>
       <c r="G38" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -3244,7 +3241,7 @@
         <v>3</v>
       </c>
       <c r="G39" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -3267,7 +3264,7 @@
         <v>3</v>
       </c>
       <c r="G40" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -3290,7 +3287,7 @@
         <v>3</v>
       </c>
       <c r="G41" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -3313,7 +3310,7 @@
         <v>3</v>
       </c>
       <c r="G42" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -3336,7 +3333,7 @@
         <v>3</v>
       </c>
       <c r="G43" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="31.5">
@@ -3359,7 +3356,7 @@
         <v>3</v>
       </c>
       <c r="G44" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -3382,7 +3379,7 @@
         <v>3</v>
       </c>
       <c r="G45" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="47.25">
@@ -3405,7 +3402,7 @@
         <v>3</v>
       </c>
       <c r="G46" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="63">
@@ -3428,7 +3425,7 @@
         <v>3</v>
       </c>
       <c r="G47" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -3451,7 +3448,7 @@
         <v>3</v>
       </c>
       <c r="G48" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -3474,7 +3471,7 @@
         <v>3</v>
       </c>
       <c r="G49" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -3497,7 +3494,7 @@
         <v>3</v>
       </c>
       <c r="G50" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -3520,7 +3517,7 @@
         <v>3</v>
       </c>
       <c r="G51" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -3543,7 +3540,7 @@
         <v>3</v>
       </c>
       <c r="G52" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -3655,7 +3652,7 @@
   <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -3686,10 +3683,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" s="40" t="s">
         <v>157</v>
-      </c>
-      <c r="G1" s="40" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -3712,7 +3709,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="40" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -3735,7 +3732,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="40" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -3758,7 +3755,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="31.5">
@@ -3781,7 +3778,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -3804,7 +3801,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -3827,7 +3824,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -3850,7 +3847,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -3873,7 +3870,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -3896,7 +3893,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -3919,7 +3916,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -3942,7 +3939,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="31.5">
@@ -3965,7 +3962,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -3988,7 +3985,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -4011,7 +4008,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -4034,7 +4031,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -4057,7 +4054,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -4080,7 +4077,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -4103,7 +4100,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -4126,7 +4123,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -4149,7 +4146,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="63">
@@ -4172,7 +4169,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -4195,7 +4192,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -4218,7 +4215,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -4241,7 +4238,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -4353,7 +4350,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G7" sqref="G1:G7"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -4383,10 +4380,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="40" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G1" s="40" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -4409,7 +4406,7 @@
         <v>4</v>
       </c>
       <c r="G2" s="40" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4432,7 +4429,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="40" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -4455,7 +4452,7 @@
         <v>4</v>
       </c>
       <c r="G4" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="31.5">
@@ -4478,7 +4475,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4501,7 +4498,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -4524,7 +4521,7 @@
         <v>4</v>
       </c>
       <c r="G7" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -4547,7 +4544,7 @@
         <v>4</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4570,7 +4567,7 @@
         <v>4</v>
       </c>
       <c r="G9" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -4593,7 +4590,7 @@
         <v>4</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -4616,7 +4613,7 @@
         <v>4</v>
       </c>
       <c r="G11" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -4639,7 +4636,7 @@
         <v>4</v>
       </c>
       <c r="G12" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="31.5">
@@ -4662,7 +4659,7 @@
         <v>4</v>
       </c>
       <c r="G13" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -4685,7 +4682,7 @@
         <v>4</v>
       </c>
       <c r="G14" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -4708,7 +4705,7 @@
         <v>4</v>
       </c>
       <c r="G15" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -4731,7 +4728,7 @@
         <v>4</v>
       </c>
       <c r="G16" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -4754,7 +4751,7 @@
         <v>4</v>
       </c>
       <c r="G17" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -4777,7 +4774,7 @@
         <v>4</v>
       </c>
       <c r="G18" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -4800,7 +4797,7 @@
         <v>4</v>
       </c>
       <c r="G19" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -4823,7 +4820,7 @@
         <v>4</v>
       </c>
       <c r="G20" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -4846,7 +4843,7 @@
         <v>4</v>
       </c>
       <c r="G21" s="40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -4962,4 +4959,1275 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97CABD2D-C77A-45CE-9C7B-8B00782490FA}">
+  <dimension ref="A1:G77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="17.625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="46" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" s="43">
+        <v>5</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="39">
+        <v>43204</v>
+      </c>
+      <c r="F3" s="41">
+        <v>5</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="F4" s="43">
+        <v>5</v>
+      </c>
+      <c r="G4" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="31.5">
+      <c r="A5" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" s="41">
+        <v>5</v>
+      </c>
+      <c r="G5" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="F6" s="43">
+        <v>5</v>
+      </c>
+      <c r="G6" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="F7" s="41">
+        <v>5</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="43">
+        <v>5</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="F9" s="41">
+        <v>5</v>
+      </c>
+      <c r="G9" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" s="43">
+        <v>5</v>
+      </c>
+      <c r="G10" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" s="41">
+        <v>5</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="43">
+        <v>5</v>
+      </c>
+      <c r="G12" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="31.5">
+      <c r="A13" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="F13" s="41">
+        <v>5</v>
+      </c>
+      <c r="G13" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="F14" s="43">
+        <v>5</v>
+      </c>
+      <c r="G14" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="F15" s="41">
+        <v>5</v>
+      </c>
+      <c r="G15" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="F16" s="43">
+        <v>5</v>
+      </c>
+      <c r="G16" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" s="41">
+        <v>5</v>
+      </c>
+      <c r="G17" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F18" s="43">
+        <v>5</v>
+      </c>
+      <c r="G18" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" s="41">
+        <v>5</v>
+      </c>
+      <c r="G19" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20" s="43">
+        <v>5</v>
+      </c>
+      <c r="G20" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="41">
+        <v>5</v>
+      </c>
+      <c r="G21" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="31.5">
+      <c r="A22" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="F22" s="43">
+        <v>5</v>
+      </c>
+      <c r="G22" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F23" s="41">
+        <v>5</v>
+      </c>
+      <c r="G23" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="31.5">
+      <c r="A24" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="F24" s="43">
+        <v>5</v>
+      </c>
+      <c r="G24" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F25" s="41">
+        <v>5</v>
+      </c>
+      <c r="G25" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F26" s="43">
+        <v>5</v>
+      </c>
+      <c r="G26" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" s="41">
+        <v>5</v>
+      </c>
+      <c r="G27" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" s="43">
+        <v>5</v>
+      </c>
+      <c r="G28" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="31.5">
+      <c r="A29" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="F29" s="41">
+        <v>5</v>
+      </c>
+      <c r="G29" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F30" s="43">
+        <v>5</v>
+      </c>
+      <c r="G30" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="63">
+      <c r="A31" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="F31" s="41">
+        <v>5</v>
+      </c>
+      <c r="G31" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F32" s="43">
+        <v>5</v>
+      </c>
+      <c r="G32" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F33" s="41">
+        <v>5</v>
+      </c>
+      <c r="G33" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F34" s="43">
+        <v>5</v>
+      </c>
+      <c r="G34" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F35" s="41">
+        <v>5</v>
+      </c>
+      <c r="G35" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F36" s="43">
+        <v>5</v>
+      </c>
+      <c r="G36" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F37" s="41">
+        <v>5</v>
+      </c>
+      <c r="G37" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F38" s="43">
+        <v>5</v>
+      </c>
+      <c r="G38" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F39" s="41">
+        <v>5</v>
+      </c>
+      <c r="G39" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F40" s="43">
+        <v>5</v>
+      </c>
+      <c r="G40" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F41" s="41">
+        <v>5</v>
+      </c>
+      <c r="G41" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F42" s="43">
+        <v>5</v>
+      </c>
+      <c r="G42" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F43" s="41">
+        <v>5</v>
+      </c>
+      <c r="G43" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="31.5">
+      <c r="A44" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="F44" s="43">
+        <v>5</v>
+      </c>
+      <c r="G44" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F45" s="41">
+        <v>5</v>
+      </c>
+      <c r="G45" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="47.25">
+      <c r="A46" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="F46" s="43">
+        <v>5</v>
+      </c>
+      <c r="G46" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="63">
+      <c r="A47" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F47" s="41">
+        <v>5</v>
+      </c>
+      <c r="G47" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48">
+        <v>5</v>
+      </c>
+      <c r="C48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F48" s="43">
+        <v>5</v>
+      </c>
+      <c r="G48" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49">
+        <v>6</v>
+      </c>
+      <c r="C49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E49" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="F49" s="41">
+        <v>5</v>
+      </c>
+      <c r="G49" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50">
+        <v>6</v>
+      </c>
+      <c r="C50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F50" s="43">
+        <v>5</v>
+      </c>
+      <c r="G50" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="16"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="16"/>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="16"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="16"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="17"/>
+      <c r="D68" s="17"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="16"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="17"/>
+      <c r="D69" s="17"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="16"/>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="16"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="17"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="16"/>
+      <c r="F70" s="16"/>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="16"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="17"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="16"/>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="16"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="17"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="16"/>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="18"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="19"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="18"/>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="18"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="19"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="18"/>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="18"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="19"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="18"/>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="18"/>
+      <c r="B76" s="19"/>
+      <c r="C76" s="19"/>
+      <c r="D76" s="19"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="18"/>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="18"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="19"/>
+      <c r="D77" s="19"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="18"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
record newtto answer to database
</commit_message>
<xml_diff>
--- a/third_party_feedback/feedback/data/eqlabels.xlsx
+++ b/third_party_feedback/feedback/data/eqlabels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\code\github\abelit-ThirdParty\third_party_feedback\feedback\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ychen\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD9C194-FC2D-4239-9236-E9F12287FB15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F16B4B-4B33-47C7-A871-279D2654E4AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TTO" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="DCE" sheetId="3" r:id="rId3"/>
     <sheet name="Open ended questions" sheetId="4" r:id="rId4"/>
     <sheet name="Non-Stopping TTO" sheetId="5" r:id="rId5"/>
+    <sheet name="New TTO" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="161">
   <si>
     <t>Presentation</t>
   </si>
@@ -1061,8 +1062,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4965,7 +4966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97CABD2D-C77A-45CE-9C7B-8B00782490FA}">
   <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F50"/>
     </sheetView>
   </sheetViews>
@@ -6230,4 +6231,1275 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A6A2DC-A179-441E-892C-258091DC427D}">
+  <dimension ref="A1:G77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="17.625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="46" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" s="43">
+        <v>6</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="39">
+        <v>43204</v>
+      </c>
+      <c r="F3" s="41">
+        <v>6</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="F4" s="43">
+        <v>6</v>
+      </c>
+      <c r="G4" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="31.5">
+      <c r="A5" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" s="41">
+        <v>6</v>
+      </c>
+      <c r="G5" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="F6" s="43">
+        <v>6</v>
+      </c>
+      <c r="G6" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="F7" s="41">
+        <v>6</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="43">
+        <v>6</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="F9" s="41">
+        <v>6</v>
+      </c>
+      <c r="G9" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" s="43">
+        <v>6</v>
+      </c>
+      <c r="G10" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" s="41">
+        <v>6</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="43">
+        <v>6</v>
+      </c>
+      <c r="G12" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="31.5">
+      <c r="A13" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="F13" s="41">
+        <v>6</v>
+      </c>
+      <c r="G13" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="F14" s="43">
+        <v>6</v>
+      </c>
+      <c r="G14" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="F15" s="41">
+        <v>6</v>
+      </c>
+      <c r="G15" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="F16" s="43">
+        <v>6</v>
+      </c>
+      <c r="G16" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" s="41">
+        <v>6</v>
+      </c>
+      <c r="G17" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F18" s="43">
+        <v>6</v>
+      </c>
+      <c r="G18" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" s="41">
+        <v>6</v>
+      </c>
+      <c r="G19" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20" s="43">
+        <v>6</v>
+      </c>
+      <c r="G20" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="41">
+        <v>6</v>
+      </c>
+      <c r="G21" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="31.5">
+      <c r="A22" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="F22" s="43">
+        <v>6</v>
+      </c>
+      <c r="G22" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F23" s="41">
+        <v>6</v>
+      </c>
+      <c r="G23" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="31.5">
+      <c r="A24" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="F24" s="43">
+        <v>6</v>
+      </c>
+      <c r="G24" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F25" s="41">
+        <v>6</v>
+      </c>
+      <c r="G25" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F26" s="43">
+        <v>6</v>
+      </c>
+      <c r="G26" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" s="41">
+        <v>6</v>
+      </c>
+      <c r="G27" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" s="43">
+        <v>6</v>
+      </c>
+      <c r="G28" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="31.5">
+      <c r="A29" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="F29" s="41">
+        <v>6</v>
+      </c>
+      <c r="G29" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F30" s="43">
+        <v>6</v>
+      </c>
+      <c r="G30" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="63">
+      <c r="A31" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="F31" s="41">
+        <v>6</v>
+      </c>
+      <c r="G31" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F32" s="43">
+        <v>6</v>
+      </c>
+      <c r="G32" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F33" s="41">
+        <v>6</v>
+      </c>
+      <c r="G33" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F34" s="43">
+        <v>6</v>
+      </c>
+      <c r="G34" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F35" s="41">
+        <v>6</v>
+      </c>
+      <c r="G35" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F36" s="43">
+        <v>6</v>
+      </c>
+      <c r="G36" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F37" s="41">
+        <v>6</v>
+      </c>
+      <c r="G37" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F38" s="43">
+        <v>6</v>
+      </c>
+      <c r="G38" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F39" s="41">
+        <v>6</v>
+      </c>
+      <c r="G39" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F40" s="43">
+        <v>6</v>
+      </c>
+      <c r="G40" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F41" s="41">
+        <v>6</v>
+      </c>
+      <c r="G41" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F42" s="43">
+        <v>6</v>
+      </c>
+      <c r="G42" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F43" s="41">
+        <v>6</v>
+      </c>
+      <c r="G43" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="31.5">
+      <c r="A44" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="F44" s="43">
+        <v>6</v>
+      </c>
+      <c r="G44" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F45" s="41">
+        <v>6</v>
+      </c>
+      <c r="G45" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="47.25">
+      <c r="A46" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="F46" s="43">
+        <v>6</v>
+      </c>
+      <c r="G46" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="63">
+      <c r="A47" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F47" s="41">
+        <v>6</v>
+      </c>
+      <c r="G47" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48">
+        <v>5</v>
+      </c>
+      <c r="C48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F48" s="43">
+        <v>6</v>
+      </c>
+      <c r="G48" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49">
+        <v>6</v>
+      </c>
+      <c r="C49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E49" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="F49" s="41">
+        <v>6</v>
+      </c>
+      <c r="G49" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50">
+        <v>6</v>
+      </c>
+      <c r="C50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F50" s="43">
+        <v>6</v>
+      </c>
+      <c r="G50" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="16"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="16"/>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="16"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="17"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="16"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="17"/>
+      <c r="D68" s="17"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="16"/>
+      <c r="B69" s="17"/>
+      <c r="C69" s="17"/>
+      <c r="D69" s="17"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="16"/>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="16"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="17"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="16"/>
+      <c r="F70" s="16"/>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="16"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="17"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="16"/>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="16"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="17"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="16"/>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="18"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="19"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="18"/>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="18"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="19"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="18"/>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="18"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="19"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="18"/>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="18"/>
+      <c r="B76" s="19"/>
+      <c r="C76" s="19"/>
+      <c r="D76" s="19"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="18"/>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="18"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="19"/>
+      <c r="D77" s="19"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="18"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>